<commit_message>
thoughts on heat flow model build-up in documentation House_model_References/lumped_element.tex
</commit_message>
<xml_diff>
--- a/housemodel/buildings/xl_for_house_buffer.xlsx
+++ b/housemodel/buildings/xl_for_house_buffer.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PROJECTS_NOVA\MCSE@BTO\FUTUREFACTORY\twozone_housemodel-git\housemodel\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denci\Documents\research\twozone_housemodel-git\housemodel\buildings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C068AD7D-40D6-49B1-8FFE-1F8D0A1A377E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCB9DBA-5D53-4D7B-9547-B95E159145B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34905" yWindow="1155" windowWidth="15630" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58560" yWindow="990" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="4" r:id="rId1"/>
     <sheet name="edges" sheetId="3" r:id="rId2"/>
     <sheet name="flows" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="House_nodes">nodes!$A$1:$D$4</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -426,23 +429,23 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A6" sqref="A6:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.140625" customWidth="1"/>
+    <col min="1" max="2" width="14.109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -458,7 +461,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -474,7 +477,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -490,7 +493,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -498,7 +501,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -508,7 +511,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -524,7 +527,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -538,7 +541,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1">
         <v>1</v>
@@ -550,7 +553,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -558,14 +561,14 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -581,7 +584,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -597,7 +600,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -605,7 +608,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -613,7 +616,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -634,16 +637,16 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -671,17 +674,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -692,7 +695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -721,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>

</xml_diff>